<commit_message>
Added a bunch of new results for synthetic instances
</commit_message>
<xml_diff>
--- a/Python/output/synthetic/FAresults.xlsx
+++ b/Python/output/synthetic/FAresults.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/local_ysong3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongjis/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/output/synthetic/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0770A247-98A6-AD44-99DC-B783DFD178AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="51160" windowHeight="24400" tabRatio="500"/>
+    <workbookView xWindow="13820" yWindow="3380" windowWidth="30920" windowHeight="18100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAresults" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -115,6 +116,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -382,11 +386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,19 +468,19 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1705.1356003737301</v>
+        <v>1693.24305923936</v>
       </c>
       <c r="K2">
-        <v>1643.8709488939701</v>
+        <v>1646.3548631072999</v>
       </c>
       <c r="L2">
-        <v>148.09023048863901</v>
+        <v>147.548791195474</v>
       </c>
       <c r="M2">
-        <v>29.016628265380799</v>
+        <v>20.072869777679401</v>
       </c>
       <c r="N2">
-        <v>1.4293529987335201</v>
+        <v>1.01221299171447</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -508,19 +512,19 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>3974.20309173333</v>
+        <v>4047.6283461951298</v>
       </c>
       <c r="K3">
-        <v>3855.24051201883</v>
+        <v>3923.31621807585</v>
       </c>
       <c r="L3">
-        <v>344.93916935272603</v>
+        <v>342.236661985284</v>
       </c>
       <c r="M3">
-        <v>42.828015089034999</v>
+        <v>40.301218986511202</v>
       </c>
       <c r="N3">
-        <v>1.6753170490264799</v>
+        <v>1.4167149066925</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -552,19 +556,19 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>8469.8189826262696</v>
+        <v>8734.3316151352501</v>
       </c>
       <c r="K4">
-        <v>8646.7367930425498</v>
+        <v>8876.3784815997096</v>
       </c>
       <c r="L4">
-        <v>1088.2438573394199</v>
+        <v>1148.0957136892</v>
       </c>
       <c r="M4">
-        <v>21.41499710083</v>
+        <v>25.666698932647702</v>
       </c>
       <c r="N4">
-        <v>1.3348491191864</v>
+        <v>1.14189624786376</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -596,19 +600,19 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>3184.9766321284001</v>
+        <v>3175.2612217728001</v>
       </c>
       <c r="K5">
-        <v>3065.9880030722002</v>
+        <v>3061.8431348905401</v>
       </c>
       <c r="L5">
-        <v>269.73928983618998</v>
+        <v>265.78450617931298</v>
       </c>
       <c r="M5">
-        <v>22.503262996673499</v>
+        <v>22.6078107357025</v>
       </c>
       <c r="N5">
-        <v>1.70457220077514</v>
+        <v>1.3583550453186</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -640,19 +644,19 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>7434.1462341775696</v>
+        <v>7590.1474748929504</v>
       </c>
       <c r="K6">
-        <v>7242.1584109677196</v>
+        <v>7391.6613365755602</v>
       </c>
       <c r="L6">
-        <v>619.17890283761506</v>
+        <v>614.06392272750804</v>
       </c>
       <c r="M6">
-        <v>55.748380184173499</v>
+        <v>42.9126200675964</v>
       </c>
       <c r="N6">
-        <v>2.11629295349121</v>
+        <v>1.7157130241394001</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -684,19 +688,19 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>16182.694199147099</v>
+        <v>16672.588923506999</v>
       </c>
       <c r="K7">
-        <v>16669.638789892699</v>
+        <v>17138.507859714999</v>
       </c>
       <c r="L7">
-        <v>1902.2380570110199</v>
+        <v>1928.8896647270899</v>
       </c>
       <c r="M7">
-        <v>42.920448064803999</v>
+        <v>26.319837808609002</v>
       </c>
       <c r="N7">
-        <v>1.9374101161956701</v>
+        <v>1.43411993980407</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -728,19 +732,19 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>4891.4295057730396</v>
+        <v>4859.5916601945601</v>
       </c>
       <c r="K8">
-        <v>4735.5177837373903</v>
+        <v>4696.1888813287896</v>
       </c>
       <c r="L8">
-        <v>421.792502425539</v>
+        <v>407.38727418102502</v>
       </c>
       <c r="M8">
-        <v>26.7885258197784</v>
+        <v>24.252118587493801</v>
       </c>
       <c r="N8">
-        <v>2.0458879470825102</v>
+        <v>1.6757788658142001</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -772,19 +776,19 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>11309.5760108457</v>
+        <v>11503.9671198536</v>
       </c>
       <c r="K9">
-        <v>10992.861335465601</v>
+        <v>11183.198500520301</v>
       </c>
       <c r="L9">
-        <v>996.25939012066306</v>
+        <v>988.94111801134704</v>
       </c>
       <c r="M9">
-        <v>57.699283123016301</v>
+        <v>50.649883031845</v>
       </c>
       <c r="N9">
-        <v>2.4139368534088099</v>
+        <v>2.0834767818450901</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -816,19 +820,19 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>23593.604446376899</v>
+        <v>24343.316618609799</v>
       </c>
       <c r="K10">
-        <v>24287.2314791764</v>
+        <v>25016.8533276081</v>
       </c>
       <c r="L10">
-        <v>2776.6422226117302</v>
+        <v>2765.2264000352702</v>
       </c>
       <c r="M10">
-        <v>25.038389921188301</v>
+        <v>19.1527469158172</v>
       </c>
       <c r="N10">
-        <v>2.0639119148254301</v>
+        <v>1.6396369934082</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -860,19 +864,19 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1965.8002758549201</v>
+        <v>1953.1143387864299</v>
       </c>
       <c r="K11">
-        <v>1964.4831295178999</v>
+        <v>1965.2384193292201</v>
       </c>
       <c r="L11">
-        <v>299.84407521214598</v>
+        <v>299.37100153792602</v>
       </c>
       <c r="M11">
-        <v>27.219316244125299</v>
+        <v>28.137087106704701</v>
       </c>
       <c r="N11">
-        <v>2.0695881843566801</v>
+        <v>1.2485949993133501</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -904,19 +908,19 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>4122.1999001628601</v>
+        <v>4192.7927102866197</v>
       </c>
       <c r="K12">
-        <v>4052.7270741137199</v>
+        <v>4118.4087810936599</v>
       </c>
       <c r="L12">
-        <v>433.65565570515503</v>
+        <v>431.42080105974401</v>
       </c>
       <c r="M12">
-        <v>51.532851934432898</v>
+        <v>43.541208982467602</v>
       </c>
       <c r="N12">
-        <v>2.3947107791900599</v>
+        <v>1.55922508239746</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -948,19 +952,19 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>8264.0267817254808</v>
+        <v>8522.4736047607694</v>
       </c>
       <c r="K13">
-        <v>8411.2452368334998</v>
+        <v>8648.0453496821192</v>
       </c>
       <c r="L13">
-        <v>1100.1952812678801</v>
+        <v>1160.09503080482</v>
       </c>
       <c r="M13">
-        <v>29.909237861633301</v>
+        <v>18.973545074462798</v>
       </c>
       <c r="N13">
-        <v>2.13689684867858</v>
+        <v>1.1587598323821999</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -992,19 +996,19 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>3329.0142864213799</v>
+        <v>3315.2955626661201</v>
       </c>
       <c r="K14">
-        <v>3199.05353355229</v>
+        <v>3202.6606796494998</v>
       </c>
       <c r="L14">
-        <v>340.16864879906399</v>
+        <v>337.812983688636</v>
       </c>
       <c r="M14">
-        <v>27.498515129089299</v>
+        <v>31.064941883087101</v>
       </c>
       <c r="N14">
-        <v>2.4005479812621999</v>
+        <v>1.64759302139282</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1036,19 +1040,19 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>7479.3441232940804</v>
+        <v>7629.6113751413004</v>
       </c>
       <c r="K15">
-        <v>7313.3655931533804</v>
+        <v>7434.9345907757697</v>
       </c>
       <c r="L15">
-        <v>660.438246446025</v>
+        <v>647.85965374569696</v>
       </c>
       <c r="M15">
-        <v>55.719377994537297</v>
+        <v>58.616178035735999</v>
       </c>
       <c r="N15">
-        <v>2.9251410961151101</v>
+        <v>2.0740659236907901</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1080,19 +1084,19 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>15733.8357439953</v>
+        <v>16214.4869545905</v>
       </c>
       <c r="K16">
-        <v>16201.9100295139</v>
+        <v>16657.4621992014</v>
       </c>
       <c r="L16">
-        <v>1916.38517934224</v>
+        <v>1943.1303286760501</v>
       </c>
       <c r="M16">
-        <v>43.026655197143498</v>
+        <v>25.836368083953801</v>
       </c>
       <c r="N16">
-        <v>2.5753369331359801</v>
+        <v>1.5968999862670801</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1124,19 +1128,19 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>5231.9408455413104</v>
+        <v>5205.69712455427</v>
       </c>
       <c r="K17">
-        <v>5058.1282644877401</v>
+        <v>5017.3542107557596</v>
       </c>
       <c r="L17">
-        <v>559.86655146211501</v>
+        <v>548.50772867839703</v>
       </c>
       <c r="M17">
-        <v>24.047222852706899</v>
+        <v>38.1137981414794</v>
       </c>
       <c r="N17">
-        <v>2.7002701759338299</v>
+        <v>2.04055571556091</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1168,19 +1172,19 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>11451.617376312999</v>
+        <v>11642.0867005615</v>
       </c>
       <c r="K18">
-        <v>11127.025560902301</v>
+        <v>11282.4036536194</v>
       </c>
       <c r="L18">
-        <v>1101.5677755366701</v>
+        <v>1069.68484653769</v>
       </c>
       <c r="M18">
-        <v>57.9039559364318</v>
+        <v>53.226900815963702</v>
       </c>
       <c r="N18">
-        <v>3.76468801498413</v>
+        <v>2.3937091827392498</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -1212,19 +1216,19 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>22980.292043670801</v>
+        <v>23723.907113613899</v>
       </c>
       <c r="K19">
-        <v>23674.700084882101</v>
+        <v>24397.3172266041</v>
       </c>
       <c r="L19">
-        <v>2792.6326035806401</v>
+        <v>2781.7244841746201</v>
       </c>
       <c r="M19">
-        <v>42.386160850524902</v>
+        <v>23.897411823272702</v>
       </c>
       <c r="N19">
-        <v>3.12760186195373</v>
+        <v>1.9083940982818599</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1256,19 +1260,19 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>1819.4497768671799</v>
+        <v>1807.3448518176899</v>
       </c>
       <c r="K20">
-        <v>1800.2324895417701</v>
+        <v>1800.9811302841099</v>
       </c>
       <c r="L20">
-        <v>224.73570353465101</v>
+        <v>223.98719762376501</v>
       </c>
       <c r="M20">
-        <v>30.862019062042201</v>
+        <v>29.5954928398132</v>
       </c>
       <c r="N20">
-        <v>3.0809881687164302</v>
+        <v>1.4088163375854399</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -1300,19 +1304,19 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>4059.4987810746202</v>
+        <v>4130.2649586979096</v>
       </c>
       <c r="K21">
-        <v>3965.6668045903002</v>
+        <v>4032.6479728908798</v>
       </c>
       <c r="L21">
-        <v>389.30081517164001</v>
+        <v>387.069209689628</v>
       </c>
       <c r="M21">
-        <v>79.410282135009695</v>
+        <v>73.338605880737305</v>
       </c>
       <c r="N21">
-        <v>3.6950559616088801</v>
+        <v>2.1226220130920401</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1344,19 +1348,19 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>8414.2875748130191</v>
+        <v>8671.5337010338899</v>
       </c>
       <c r="K22">
-        <v>8456.3219203987901</v>
+        <v>8683.2959693764496</v>
       </c>
       <c r="L22">
-        <v>1135.4067691392199</v>
+        <v>1191.9036571106001</v>
       </c>
       <c r="M22">
-        <v>55.131071805953901</v>
+        <v>25.123516798019399</v>
       </c>
       <c r="N22">
-        <v>3.21880674362182</v>
+        <v>1.4025638103485101</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -1388,19 +1392,19 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>3263.3912814138798</v>
+        <v>3249.1254220975902</v>
       </c>
       <c r="K23">
-        <v>3056.2054991024302</v>
+        <v>3058.2804706983602</v>
       </c>
       <c r="L23">
-        <v>270.02240692275501</v>
+        <v>267.02864930987101</v>
       </c>
       <c r="M23">
-        <v>36.0731809139251</v>
+        <v>39.744082927703801</v>
       </c>
       <c r="N23">
-        <v>3.38308405876159</v>
+        <v>1.8805849552154501</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -1432,19 +1436,19 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>7512.6596778469602</v>
+        <v>7662.5589920053499</v>
       </c>
       <c r="K24">
-        <v>7266.9200557383801</v>
+        <v>7422.8573422867403</v>
       </c>
       <c r="L24">
-        <v>634.58223636331695</v>
+        <v>632.23653259841103</v>
       </c>
       <c r="M24">
-        <v>105.08026289939799</v>
+        <v>92.830470800399695</v>
       </c>
       <c r="N24">
-        <v>4.2685480117797798</v>
+        <v>2.6520447731018</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1476,19 +1480,19 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>15978.4608221617</v>
+        <v>16463.2760050262</v>
       </c>
       <c r="K25">
-        <v>16272.266048904999</v>
+        <v>16734.222885795902</v>
       </c>
       <c r="L25">
-        <v>1970.39393503573</v>
+        <v>1997.1584418381599</v>
       </c>
       <c r="M25">
-        <v>54.653835773468003</v>
+        <v>54.048429012298499</v>
       </c>
       <c r="N25">
-        <v>3.8599669933318999</v>
+        <v>2.1482870578765798</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -1520,19 +1524,19 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>5044.0252406701902</v>
+        <v>5021.9371284504796</v>
       </c>
       <c r="K26">
-        <v>4840.0780413476996</v>
+        <v>4788.4778933853804</v>
       </c>
       <c r="L26">
-        <v>455.389805533691</v>
+        <v>437.73767669662402</v>
       </c>
       <c r="M26">
-        <v>32.820415019988999</v>
+        <v>48.733216047286902</v>
       </c>
       <c r="N26">
-        <v>3.8222861289978001</v>
+        <v>2.4034018516540501</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -1564,19 +1568,19 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>11447.253296933701</v>
+        <v>11639.2312889356</v>
       </c>
       <c r="K27">
-        <v>11140.2053867748</v>
+        <v>11310.093409134201</v>
       </c>
       <c r="L27">
-        <v>1096.1428175316</v>
+        <v>1075.8144899644301</v>
       </c>
       <c r="M27">
-        <v>92.617938041686998</v>
+        <v>75.776366710662799</v>
       </c>
       <c r="N27">
-        <v>4.6633238792419398</v>
+        <v>2.9155290126800502</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -1608,19 +1612,19 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>23274.7569728696</v>
+        <v>24019.305581490102</v>
       </c>
       <c r="K28">
-        <v>23959.862756850402</v>
+        <v>24684.479965470699</v>
       </c>
       <c r="L28">
-        <v>2856.9879989278902</v>
+        <v>2846.36186956339</v>
       </c>
       <c r="M28">
-        <v>47.608272314071598</v>
+        <v>30.1767258644104</v>
       </c>
       <c r="N28">
-        <v>4.2401659488677899</v>
+        <v>2.1950578689575102</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1652,19 +1656,19 @@
         <v>2</v>
       </c>
       <c r="J29">
-        <v>2420.52818202545</v>
+        <v>2422.08410534326</v>
       </c>
       <c r="K29">
-        <v>2342.6132381274501</v>
+        <v>2344.3148068481801</v>
       </c>
       <c r="L29">
-        <v>201.922296543009</v>
+        <v>197.54580433881</v>
       </c>
       <c r="M29">
-        <v>25.192884922027499</v>
+        <v>25.253631114959699</v>
       </c>
       <c r="N29">
-        <v>1.3872587680816599</v>
+        <v>1.5994598865509</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -1696,19 +1700,19 @@
         <v>2</v>
       </c>
       <c r="J30">
-        <v>3110.1582020764299</v>
+        <v>3123.69977828423</v>
       </c>
       <c r="K30">
-        <v>2991.6963134860898</v>
+        <v>3000.6958551837502</v>
       </c>
       <c r="L30">
-        <v>278.35345615562602</v>
+        <v>277.54828722440197</v>
       </c>
       <c r="M30">
-        <v>30.391810894012401</v>
+        <v>28.1092641353607</v>
       </c>
       <c r="N30">
-        <v>1.48929786682128</v>
+        <v>1.6470091342926001</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -1740,19 +1744,19 @@
         <v>2</v>
       </c>
       <c r="J31">
-        <v>3790.0785181978899</v>
+        <v>3811.9235870604002</v>
       </c>
       <c r="K31">
-        <v>3790.9030776068598</v>
+        <v>3806.60557464457</v>
       </c>
       <c r="L31">
-        <v>612.11217952539403</v>
+        <v>609.41652458354201</v>
       </c>
       <c r="M31">
-        <v>49.814176082610999</v>
+        <v>25.156312227249099</v>
       </c>
       <c r="N31">
-        <v>1.74743199348449</v>
+        <v>1.60082912445068</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -1784,19 +1788,19 @@
         <v>2</v>
       </c>
       <c r="J32">
-        <v>4482.5410272839399</v>
+        <v>4494.8317499613504</v>
       </c>
       <c r="K32">
-        <v>4328.5836244804505</v>
+        <v>4345.6201745606704</v>
       </c>
       <c r="L32">
-        <v>395.09167283288599</v>
+        <v>393.14319828245101</v>
       </c>
       <c r="M32">
-        <v>38.796642065048196</v>
+        <v>30.992506265640198</v>
       </c>
       <c r="N32">
-        <v>1.90325999259948</v>
+        <v>2.0870909690856898</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -1828,19 +1832,19 @@
         <v>2</v>
       </c>
       <c r="J33">
-        <v>5814.1397631728396</v>
+        <v>5851.24457611239</v>
       </c>
       <c r="K33">
-        <v>5660.3177360074596</v>
+        <v>5736.1584883417299</v>
       </c>
       <c r="L33">
-        <v>601.43687410039001</v>
+        <v>614.19297335490205</v>
       </c>
       <c r="M33">
-        <v>51.22869515419</v>
+        <v>32.5537140369415</v>
       </c>
       <c r="N33">
-        <v>2.1420350074768</v>
+        <v>2.0754590034484801</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -1872,19 +1876,19 @@
         <v>2</v>
       </c>
       <c r="J34">
-        <v>7255.1666210159901</v>
+        <v>7305.5863152415504</v>
       </c>
       <c r="K34">
-        <v>7389.3434591499099</v>
+        <v>7464.6550936250796</v>
       </c>
       <c r="L34">
-        <v>1089.1899778075699</v>
+        <v>1225.8156541430701</v>
       </c>
       <c r="M34">
-        <v>49.098992109298699</v>
+        <v>34.487572193145702</v>
       </c>
       <c r="N34">
-        <v>2.0389120578765798</v>
+        <v>2.15663313865661</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -1916,19 +1920,19 @@
         <v>2</v>
       </c>
       <c r="J35">
-        <v>6831.5305215664903</v>
+        <v>6852.3013802126598</v>
       </c>
       <c r="K35">
-        <v>6572.5392296495202</v>
+        <v>6598.4898490158703</v>
       </c>
       <c r="L35">
-        <v>600.335291505231</v>
+        <v>598.51194090106503</v>
       </c>
       <c r="M35">
-        <v>33.250907182693403</v>
+        <v>36.203866243362398</v>
       </c>
       <c r="N35">
-        <v>2.1777441501617401</v>
+        <v>2.5928819179534899</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -1960,19 +1964,19 @@
         <v>2</v>
       </c>
       <c r="J36">
-        <v>8817.4261422531199</v>
+        <v>8859.3828983778803</v>
       </c>
       <c r="K36">
-        <v>8889.4348288005804</v>
+        <v>8960.5096218691706</v>
       </c>
       <c r="L36">
-        <v>1140.84777326482</v>
+        <v>1137.3547398964799</v>
       </c>
       <c r="M36">
-        <v>41.214429855346602</v>
+        <v>36.171231985092099</v>
       </c>
       <c r="N36">
-        <v>2.2552459239959699</v>
+        <v>2.56674003601074</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -2004,19 +2008,19 @@
         <v>2</v>
       </c>
       <c r="J37">
-        <v>10701.592018274599</v>
+        <v>10781.112821045601</v>
       </c>
       <c r="K37">
-        <v>11000.026702454699</v>
+        <v>11110.3220869375</v>
       </c>
       <c r="L37">
-        <v>1634.58211718251</v>
+        <v>1869.0612287314</v>
       </c>
       <c r="M37">
-        <v>47.031980037689202</v>
+        <v>38.465617179870598</v>
       </c>
       <c r="N37">
-        <v>2.3272080421447701</v>
+        <v>2.5690920352935702</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -2048,19 +2052,19 @@
         <v>2</v>
       </c>
       <c r="J38">
-        <v>2635.3308912458401</v>
+        <v>2636.6712396115799</v>
       </c>
       <c r="K38">
-        <v>2641.7407204219498</v>
+        <v>2642.0571728187001</v>
       </c>
       <c r="L38">
-        <v>332.40842438412699</v>
+        <v>329.34798538310099</v>
       </c>
       <c r="M38">
-        <v>33.7234721183776</v>
+        <v>29.888416051864599</v>
       </c>
       <c r="N38">
-        <v>2.1420249938964799</v>
+        <v>2.2937359809875399</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -2092,19 +2096,19 @@
         <v>2</v>
       </c>
       <c r="J39">
-        <v>3284.0732436553399</v>
+        <v>3292.31429762267</v>
       </c>
       <c r="K39">
-        <v>3227.0857216939899</v>
+        <v>3223.5649920819701</v>
       </c>
       <c r="L39">
-        <v>388.72009361113999</v>
+        <v>385.36669756232601</v>
       </c>
       <c r="M39">
-        <v>48.158479690551701</v>
+        <v>36.376519203186</v>
       </c>
       <c r="N39">
-        <v>2.2923569679260201</v>
+        <v>2.3813500404357901</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -2136,19 +2140,19 @@
         <v>2</v>
       </c>
       <c r="J40">
-        <v>3920.2973682618999</v>
+        <v>3936.1189365233299</v>
       </c>
       <c r="K40">
-        <v>3969.5149392027802</v>
+        <v>3971.2709525506598</v>
       </c>
       <c r="L40">
-        <v>668.12283856712997</v>
+        <v>665.85121048069402</v>
       </c>
       <c r="M40">
-        <v>36.452404022216797</v>
+        <v>24.537326812744102</v>
       </c>
       <c r="N40">
-        <v>2.1943302154540998</v>
+        <v>2.2004690170288002</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -2180,19 +2184,19 @@
         <v>2</v>
       </c>
       <c r="J41">
-        <v>4582.2626357515801</v>
+        <v>4589.5710572607604</v>
       </c>
       <c r="K41">
-        <v>4479.2232588495099</v>
+        <v>4494.5973145892303</v>
       </c>
       <c r="L41">
-        <v>449.29448891758602</v>
+        <v>447.23641742167302</v>
       </c>
       <c r="M41">
-        <v>37.2958438396453</v>
+        <v>44.5311408042907</v>
       </c>
       <c r="N41">
-        <v>2.5239937305450399</v>
+        <v>2.9235448837280198</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -2224,19 +2228,19 @@
         <v>2</v>
       </c>
       <c r="J42">
-        <v>5855.2413040439696</v>
+        <v>5888.8925165209703</v>
       </c>
       <c r="K42">
-        <v>5748.40547267688</v>
+        <v>5791.7229785672298</v>
       </c>
       <c r="L42">
-        <v>636.693859799449</v>
+        <v>636.50307542779103</v>
       </c>
       <c r="M42">
-        <v>44.028871774673398</v>
+        <v>35.272660970687802</v>
       </c>
       <c r="N42">
-        <v>2.63854908943176</v>
+        <v>2.86497902870178</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -2268,19 +2272,19 @@
         <v>2</v>
       </c>
       <c r="J43">
-        <v>7205.6704839904896</v>
+        <v>7252.0324421619998</v>
       </c>
       <c r="K43">
-        <v>7375.1619523566596</v>
+        <v>7436.53531192628</v>
       </c>
       <c r="L43">
-        <v>1105.8784067295101</v>
+        <v>1238.4509994602799</v>
       </c>
       <c r="M43">
-        <v>42.909720182418802</v>
+        <v>39.835301876068101</v>
       </c>
       <c r="N43">
-        <v>2.6909618377685498</v>
+        <v>2.90826320648193</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -2312,19 +2316,19 @@
         <v>2</v>
       </c>
       <c r="J44">
-        <v>7097.3382612722298</v>
+        <v>7114.9479955328798</v>
       </c>
       <c r="K44">
-        <v>6841.0678205268296</v>
+        <v>6855.9005597943096</v>
       </c>
       <c r="L44">
-        <v>698.30697321439402</v>
+        <v>695.75531951322398</v>
       </c>
       <c r="M44">
-        <v>44.2179400920867</v>
+        <v>43.021525144576998</v>
       </c>
       <c r="N44">
-        <v>2.9667997360229399</v>
+        <v>3.3412199020385698</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -2356,19 +2360,19 @@
         <v>2</v>
       </c>
       <c r="J45">
-        <v>8980.3385232934907</v>
+        <v>9021.6606865008707</v>
       </c>
       <c r="K45">
-        <v>8996.4480181326508</v>
+        <v>9059.7497174707896</v>
       </c>
       <c r="L45">
-        <v>1177.4017428990601</v>
+        <v>1176.04175822049</v>
       </c>
       <c r="M45">
-        <v>48.570221185684197</v>
+        <v>44.163291931152301</v>
       </c>
       <c r="N45">
-        <v>3.0147280693054199</v>
+        <v>3.40865802764892</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -2400,19 +2404,19 @@
         <v>2</v>
       </c>
       <c r="J46">
-        <v>10734.3404044982</v>
+        <v>10810.4202445764</v>
       </c>
       <c r="K46">
-        <v>11066.004371548799</v>
+        <v>11146.417992741</v>
       </c>
       <c r="L46">
-        <v>1668.50317329068</v>
+        <v>1897.13379340612</v>
       </c>
       <c r="M46">
-        <v>53.123578310012803</v>
+        <v>62.675053834915097</v>
       </c>
       <c r="N46">
-        <v>3.0502169132232599</v>
+        <v>3.59109187126159</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -2444,19 +2448,19 @@
         <v>2</v>
       </c>
       <c r="J47">
-        <v>2515.2601592480901</v>
+        <v>2516.8658270003102</v>
       </c>
       <c r="K47">
-        <v>2486.0304967621501</v>
+        <v>2486.8370573552702</v>
       </c>
       <c r="L47">
-        <v>263.39594165856403</v>
+        <v>259.63802800687699</v>
       </c>
       <c r="M47">
-        <v>77.686182737350407</v>
+        <v>41.399219036102203</v>
       </c>
       <c r="N47">
-        <v>3.5656180381774898</v>
+        <v>3.3611710071563698</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -2488,19 +2492,19 @@
         <v>2</v>
       </c>
       <c r="J48">
-        <v>3211.64593375596</v>
+        <v>3222.3581769379898</v>
       </c>
       <c r="K48">
-        <v>3141.9565928832399</v>
+        <v>3133.6263662207798</v>
       </c>
       <c r="L48">
-        <v>335.45067510906603</v>
+        <v>330.74979208306098</v>
       </c>
       <c r="M48">
-        <v>60.8195509910583</v>
+        <v>64.682331085205007</v>
       </c>
       <c r="N48">
-        <v>3.3570189476013099</v>
+        <v>3.7002370357513401</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -2532,19 +2536,19 @@
         <v>2</v>
       </c>
       <c r="J49">
-        <v>3891.1721304064299</v>
+        <v>3909.7710246778101</v>
       </c>
       <c r="K49">
-        <v>3924.3868428145001</v>
+        <v>3935.0163266897898</v>
       </c>
       <c r="L49">
-        <v>641.34083848617104</v>
+        <v>641.22049945477204</v>
       </c>
       <c r="M49">
-        <v>61.2600708007812</v>
+        <v>54.9283640384674</v>
       </c>
       <c r="N49">
-        <v>3.3647220134735099</v>
+        <v>3.6364059448242099</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -2576,19 +2580,19 @@
         <v>2</v>
       </c>
       <c r="J50">
-        <v>4552.8783469309601</v>
+        <v>4559.8560908535201</v>
       </c>
       <c r="K50">
-        <v>4378.2285465230298</v>
+        <v>4393.2327337475799</v>
       </c>
       <c r="L50">
-        <v>406.78668938448698</v>
+        <v>404.47473655363598</v>
       </c>
       <c r="M50">
-        <v>50.513803005218499</v>
+        <v>63.627943992614703</v>
       </c>
       <c r="N50">
-        <v>3.6951160430908199</v>
+        <v>4.1367378234863201</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
@@ -2620,19 +2624,19 @@
         <v>2</v>
       </c>
       <c r="J51">
-        <v>5881.0943737930402</v>
+        <v>5915.0570457694103</v>
       </c>
       <c r="K51">
-        <v>5706.8550800141502</v>
+        <v>5749.1011672997702</v>
       </c>
       <c r="L51">
-        <v>612.45197909995204</v>
+        <v>612.04088299344801</v>
       </c>
       <c r="M51">
-        <v>66.214990854263306</v>
+        <v>70.027151107788001</v>
       </c>
       <c r="N51">
-        <v>3.7707700729370099</v>
+        <v>4.2036850452423096</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -2664,19 +2668,19 @@
         <v>2</v>
       </c>
       <c r="J52">
-        <v>7289.0655644627304</v>
+        <v>7339.44580624226</v>
       </c>
       <c r="K52">
-        <v>7404.4492772635103</v>
+        <v>7451.6578839725898</v>
       </c>
       <c r="L52">
-        <v>1095.9503978625901</v>
+        <v>1222.20407310479</v>
       </c>
       <c r="M52">
-        <v>95.047540187835693</v>
+        <v>68.078272104263306</v>
       </c>
       <c r="N52">
-        <v>4.0573439598083496</v>
+        <v>4.1951529979705802</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -2708,19 +2712,19 @@
         <v>2</v>
       </c>
       <c r="J53">
-        <v>6977.5464396418301</v>
+        <v>6994.9871313817503</v>
       </c>
       <c r="K53">
-        <v>6684.8686611390203</v>
+        <v>6701.9952792203303</v>
       </c>
       <c r="L53">
-        <v>627.46394168725999</v>
+        <v>624.77578025761898</v>
       </c>
       <c r="M53">
-        <v>52.318528890609699</v>
+        <v>48.015896081924403</v>
       </c>
       <c r="N53">
-        <v>3.9019031524658199</v>
+        <v>4.4885289669036803</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -2752,19 +2756,19 @@
         <v>2</v>
       </c>
       <c r="J54">
-        <v>8939.7698003815894</v>
+        <v>8983.2399836875102</v>
       </c>
       <c r="K54">
-        <v>8952.9813051996098</v>
+        <v>9021.0029857380505</v>
       </c>
       <c r="L54">
-        <v>1151.7033462142999</v>
+        <v>1150.3886051176701</v>
       </c>
       <c r="M54">
-        <v>93.377465009689303</v>
+        <v>54.745103836059499</v>
       </c>
       <c r="N54">
-        <v>4.3945608139037997</v>
+        <v>4.5465011596679599</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -2796,19 +2800,19 @@
         <v>2</v>
       </c>
       <c r="J55">
-        <v>10774.443183940401</v>
+        <v>10849.928375961499</v>
       </c>
       <c r="K55">
-        <v>11082.4672793339</v>
+        <v>11168.1402369023</v>
       </c>
       <c r="L55">
-        <v>1653.4045812065899</v>
+        <v>1876.2031724425899</v>
       </c>
       <c r="M55">
-        <v>66.618457078933702</v>
+        <v>45.109338998794499</v>
       </c>
       <c r="N55">
-        <v>4.2347218990325901</v>
+        <v>4.4181361198425204</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -2840,19 +2844,19 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1761.8786809805699</v>
+        <v>1754.98774780441</v>
       </c>
       <c r="K56">
-        <v>1763.4593083836501</v>
+        <v>1744.9561632607699</v>
       </c>
       <c r="L56">
-        <v>184.700935328425</v>
+        <v>182.73063863920399</v>
       </c>
       <c r="M56">
-        <v>319.17966103553698</v>
+        <v>138.71586894988999</v>
       </c>
       <c r="N56">
-        <v>1.41159391403198</v>
+        <v>1.0163280963897701</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -2884,19 +2888,19 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>2953.7602925158799</v>
+        <v>2986.9747487775398</v>
       </c>
       <c r="K57">
-        <v>2995.14512440722</v>
+        <v>3040.4213709032001</v>
       </c>
       <c r="L57">
-        <v>255.91928864122201</v>
+        <v>256.15240958341099</v>
       </c>
       <c r="M57">
-        <v>536.19065499305702</v>
+        <v>203.862577915191</v>
       </c>
       <c r="N57">
-        <v>1.72436094284057</v>
+        <v>1.1882960796356199</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -2928,19 +2932,19 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>6119.9507496793403</v>
+        <v>6219.4754513102398</v>
       </c>
       <c r="K58">
-        <v>5868.2419735850399</v>
+        <v>6011.9450841383004</v>
       </c>
       <c r="L58">
-        <v>730.62634425315696</v>
+        <v>740.52642810731402</v>
       </c>
       <c r="M58">
-        <v>125.925343036651</v>
+        <v>176.48017191886899</v>
       </c>
       <c r="N58">
-        <v>1.03333091735839</v>
+        <v>1.0945861339569001</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -2972,19 +2976,19 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>3330.2954412900199</v>
+        <v>3324.0617305083101</v>
       </c>
       <c r="K59">
-        <v>3350.14486042001</v>
+        <v>3332.0017242221102</v>
       </c>
       <c r="L59">
-        <v>296.30444943296197</v>
+        <v>293.66156598511202</v>
       </c>
       <c r="M59">
-        <v>246.142634153366</v>
+        <v>238.080338954925</v>
       </c>
       <c r="N59">
-        <v>1.4858260154724099</v>
+        <v>1.4870388507843</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -3016,19 +3020,19 @@
         <v>0</v>
       </c>
       <c r="J60">
-        <v>5522.2809324915197</v>
+        <v>5599.8285620352499</v>
       </c>
       <c r="K60">
-        <v>5475.2264742923999</v>
+        <v>5561.4821830930596</v>
       </c>
       <c r="L60">
-        <v>433.64524777245498</v>
+        <v>437.44760235126699</v>
       </c>
       <c r="M60">
-        <v>235.83711791038499</v>
+        <v>215.068766832351</v>
       </c>
       <c r="N60">
-        <v>1.465576171875</v>
+        <v>1.4033889770507799</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -3060,19 +3064,19 @@
         <v>0</v>
       </c>
       <c r="J61">
-        <v>11667.4897317553</v>
+        <v>11909.725115424601</v>
       </c>
       <c r="K61">
-        <v>11262.6697560674</v>
+        <v>11486.0015588392</v>
       </c>
       <c r="L61">
-        <v>1290.21351446792</v>
+        <v>1286.56647443717</v>
       </c>
       <c r="M61">
-        <v>115.769577026367</v>
+        <v>121.590980768203</v>
       </c>
       <c r="N61">
-        <v>1.2324359416961601</v>
+        <v>1.17420101165771</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -3104,19 +3108,19 @@
         <v>0</v>
       </c>
       <c r="J62">
-        <v>5118.2435568811798</v>
+        <v>5109.4741815461502</v>
       </c>
       <c r="K62">
-        <v>5165.6481343206497</v>
+        <v>5123.1076105899501</v>
       </c>
       <c r="L62">
-        <v>447.14850324435002</v>
+        <v>437.48193350762699</v>
       </c>
       <c r="M62">
-        <v>271.92933893203701</v>
+        <v>216.690898180007</v>
       </c>
       <c r="N62">
-        <v>1.88263511657714</v>
+        <v>1.60986399650573</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -3148,19 +3152,19 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>8411.6907267159804</v>
+        <v>8526.07967117933</v>
       </c>
       <c r="K63">
-        <v>8517.7178454382793</v>
+        <v>8639.2238009483808</v>
       </c>
       <c r="L63">
-        <v>712.94832642552603</v>
+        <v>713.71200184365705</v>
       </c>
       <c r="M63">
-        <v>277.97194290161099</v>
+        <v>178.77014517784099</v>
       </c>
       <c r="N63">
-        <v>1.9150578975677399</v>
+        <v>1.49000191688537</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -3192,19 +3196,19 @@
         <v>0</v>
       </c>
       <c r="J64">
-        <v>17380.811150092301</v>
+        <v>17626.309393109299</v>
       </c>
       <c r="K64">
-        <v>16694.0465249679</v>
+        <v>17208.066940579702</v>
       </c>
       <c r="L64">
-        <v>2157.5039764929102</v>
+        <v>2214.01407268802</v>
       </c>
       <c r="M64">
-        <v>170.42892694473201</v>
+        <v>183.520205974578</v>
       </c>
       <c r="N64">
-        <v>1.5645120143890301</v>
+        <v>1.5028948783874501</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -3236,19 +3240,19 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>1865.4165336543499</v>
+        <v>1855.76212573267</v>
       </c>
       <c r="K65">
-        <v>1819.3669744358599</v>
+        <v>1797.28457731545</v>
       </c>
       <c r="L65">
-        <v>213.28752634155299</v>
+        <v>210.846835889435</v>
       </c>
       <c r="M65">
-        <v>242.1635119915</v>
+        <v>222.93166589736899</v>
       </c>
       <c r="N65">
-        <v>1.7495801448821999</v>
+        <v>1.34628105163574</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -3280,19 +3284,19 @@
         <v>0</v>
       </c>
       <c r="J66">
-        <v>3003.8593359944798</v>
+        <v>3038.7058737992302</v>
       </c>
       <c r="K66">
-        <v>3000.3082381479398</v>
+        <v>3039.3461801697499</v>
       </c>
       <c r="L66">
-        <v>272.49411829860298</v>
+        <v>271.04283306197698</v>
       </c>
       <c r="M66">
-        <v>326.81777572631802</v>
+        <v>198.531777143478</v>
       </c>
       <c r="N66">
-        <v>1.8908669948577801</v>
+        <v>1.2637970447540201</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -3324,19 +3328,19 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <v>5949.8845522279898</v>
+        <v>6048.3808618683197</v>
       </c>
       <c r="K67">
-        <v>5672.0046905413101</v>
+        <v>5790.8865010479503</v>
       </c>
       <c r="L67">
-        <v>728.97815871249702</v>
+        <v>731.53852860660197</v>
       </c>
       <c r="M67">
-        <v>275.49009275436401</v>
+        <v>320.77564406394902</v>
       </c>
       <c r="N67">
-        <v>1.82319211959838</v>
+        <v>1.5614330768585201</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -3368,19 +3372,19 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <v>3349.89145995942</v>
+        <v>3370.0033901265501</v>
       </c>
       <c r="K68">
-        <v>3436.8861961482198</v>
+        <v>3334.5952821595301</v>
       </c>
       <c r="L68">
-        <v>383.52613094946997</v>
+        <v>302.38912205002299</v>
       </c>
       <c r="M68">
-        <v>185.10628581047001</v>
+        <v>179.32365489006</v>
       </c>
       <c r="N68">
-        <v>1.88231897354125</v>
+        <v>1.4685490131378101</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -3412,19 +3416,19 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>5517.5548096865105</v>
+        <v>5594.5573533090501</v>
       </c>
       <c r="K69">
-        <v>5435.5512030762002</v>
+        <v>5520.1479605254999</v>
       </c>
       <c r="L69">
-        <v>431.89987342662698</v>
+        <v>429.93875111879902</v>
       </c>
       <c r="M69">
-        <v>303.13013792037901</v>
+        <v>287.19284772872902</v>
       </c>
       <c r="N69">
-        <v>2.3350570201873699</v>
+        <v>1.7658438682556099</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -3456,19 +3460,19 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>11326.7700973179</v>
+        <v>11549.4799150871</v>
       </c>
       <c r="K70">
-        <v>10833.2885900491</v>
+        <v>11085.3234615008</v>
       </c>
       <c r="L70">
-        <v>1272.70364915344</v>
+        <v>1277.45992065359</v>
       </c>
       <c r="M70">
-        <v>407.98968887329102</v>
+        <v>570.51058411598206</v>
       </c>
       <c r="N70">
-        <v>2.5367112159728999</v>
+        <v>2.32118391990661</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -3500,19 +3504,19 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>5255.1164878995296</v>
+        <v>5241.1450716550098</v>
       </c>
       <c r="K71">
-        <v>5222.8308838811899</v>
+        <v>5152.0509335383103</v>
       </c>
       <c r="L71">
-        <v>477.70469067198201</v>
+        <v>461.57211008584397</v>
       </c>
       <c r="M71">
-        <v>259.37256073951698</v>
+        <v>277.47575616836502</v>
       </c>
       <c r="N71">
-        <v>2.232843875885</v>
+        <v>2.0754029750823899</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -3544,19 +3548,19 @@
         <v>0</v>
       </c>
       <c r="J72">
-        <v>8453.6489340144999</v>
+        <v>8553.6681332502594</v>
       </c>
       <c r="K72">
-        <v>8456.1899768193998</v>
+        <v>8578.6640167042206</v>
       </c>
       <c r="L72">
-        <v>711.73422670319906</v>
+        <v>710.75727440256799</v>
       </c>
       <c r="M72">
-        <v>296.90961265563902</v>
+        <v>221.03959608078</v>
       </c>
       <c r="N72">
-        <v>2.2482879161834699</v>
+        <v>1.7720267772674501</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -3588,19 +3592,19 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>16902.2294032352</v>
+        <v>17179.464382513401</v>
       </c>
       <c r="K73">
-        <v>16167.658092367399</v>
+        <v>16539.881465835999</v>
       </c>
       <c r="L73">
-        <v>2152.9264263729901</v>
+        <v>2166.1418338916301</v>
       </c>
       <c r="M73">
-        <v>457.124476909637</v>
+        <v>230.39122295379599</v>
       </c>
       <c r="N73">
-        <v>2.6345629692077601</v>
+        <v>1.7524168491363501</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -3632,19 +3636,19 @@
         <v>0</v>
       </c>
       <c r="J74">
-        <v>1808.50747635931</v>
+        <v>1798.8841160842901</v>
       </c>
       <c r="K74">
-        <v>1790.2334994861999</v>
+        <v>1767.2433558538901</v>
       </c>
       <c r="L74">
-        <v>197.81870955270199</v>
+        <v>193.72344604322799</v>
       </c>
       <c r="M74">
-        <v>334.22333502769402</v>
+        <v>447.73497915267899</v>
       </c>
       <c r="N74">
-        <v>2.6132349967956499</v>
+        <v>2.1063199043273899</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -3676,19 +3680,19 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>2978.8855296997699</v>
+        <v>3014.951156909</v>
       </c>
       <c r="K75">
-        <v>2992.1475901519798</v>
+        <v>3036.3096306269599</v>
       </c>
       <c r="L75">
-        <v>258.891716371195</v>
+        <v>259.07592669836902</v>
       </c>
       <c r="M75">
-        <v>312.752428054809</v>
+        <v>313.63258910179098</v>
       </c>
       <c r="N75">
-        <v>2.5881211757659899</v>
+        <v>1.7523219585418699</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -3720,19 +3724,19 @@
         <v>0</v>
       </c>
       <c r="J76">
-        <v>6015.5814283155096</v>
+        <v>6118.9464846754399</v>
       </c>
       <c r="K76">
-        <v>5732.2005421957401</v>
+        <v>5826.0640616471601</v>
       </c>
       <c r="L76">
-        <v>743.14211441339603</v>
+        <v>740.44514949074596</v>
       </c>
       <c r="M76">
-        <v>228.52557897567701</v>
+        <v>195.14518928527801</v>
       </c>
       <c r="N76">
-        <v>2.3544292449951101</v>
+        <v>1.3786361217498699</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -3764,19 +3768,19 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>3358.93943728865</v>
+        <v>3348.8916710265999</v>
       </c>
       <c r="K77">
-        <v>3356.3577311428899</v>
+        <v>3330.0246974499801</v>
       </c>
       <c r="L77">
-        <v>298.50843577018099</v>
+        <v>293.83470850319799</v>
       </c>
       <c r="M77">
-        <v>324.03716564178399</v>
+        <v>219.42978787422101</v>
       </c>
       <c r="N77">
-        <v>2.8146271705627401</v>
+        <v>1.72448801994323</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -3808,19 +3812,19 @@
         <v>0</v>
       </c>
       <c r="J78">
-        <v>5536.3474549696002</v>
+        <v>5613.1657942128304</v>
       </c>
       <c r="K78">
-        <v>5462.70781230389</v>
+        <v>5550.9584601610904</v>
       </c>
       <c r="L78">
-        <v>437.18715294187899</v>
+        <v>436.232116582873</v>
       </c>
       <c r="M78">
-        <v>445.24674320220902</v>
+        <v>430.59844398498501</v>
       </c>
       <c r="N78">
-        <v>3.0222110748290998</v>
+        <v>2.2877309322357098</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -3852,19 +3856,19 @@
         <v>0</v>
       </c>
       <c r="J79">
-        <v>11423.0701410609</v>
+        <v>11632.719678654999</v>
       </c>
       <c r="K79">
-        <v>10894.840267128</v>
+        <v>11168.1770252921</v>
       </c>
       <c r="L79">
-        <v>1284.2238277083</v>
+        <v>1293.14812228031</v>
       </c>
       <c r="M79">
-        <v>368.05669617652802</v>
+        <v>261.81256794929499</v>
       </c>
       <c r="N79">
-        <v>3.3453781604766801</v>
+        <v>1.75774073600769</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -3896,19 +3900,19 @@
         <v>0</v>
       </c>
       <c r="J80">
-        <v>5186.1950232404097</v>
+        <v>5173.1499405052</v>
       </c>
       <c r="K80">
-        <v>5195.4856530272</v>
+        <v>5143.2219707863796</v>
       </c>
       <c r="L80">
-        <v>460.06582438174399</v>
+        <v>449.41134047452402</v>
       </c>
       <c r="M80">
-        <v>263.36980295181201</v>
+        <v>287.76785492897</v>
       </c>
       <c r="N80">
-        <v>3.0272090435028001</v>
+        <v>2.1873688697814901</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -3940,19 +3944,19 @@
         <v>0</v>
       </c>
       <c r="J81">
-        <v>8457.1747486899803</v>
+        <v>8563.0900698237092</v>
       </c>
       <c r="K81">
-        <v>8512.0024643925299</v>
+        <v>8630.1234818114408</v>
       </c>
       <c r="L81">
-        <v>719.11636295449296</v>
+        <v>717.61287302324195</v>
       </c>
       <c r="M81">
-        <v>495.33272409439002</v>
+        <v>499.11554217338499</v>
       </c>
       <c r="N81">
-        <v>3.5214393138885498</v>
+        <v>2.7312598228454501</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -3984,19 +3988,19 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <v>16989.053518408</v>
+        <v>17279.528416526799</v>
       </c>
       <c r="K82">
-        <v>16246.2524157076</v>
+        <v>16531.8461879227</v>
       </c>
       <c r="L82">
-        <v>2172.0010304820398</v>
+        <v>2165.7710284278701</v>
       </c>
       <c r="M82">
-        <v>397.88393807411097</v>
+        <v>252.80678200721701</v>
       </c>
       <c r="N82">
-        <v>3.3679628372192298</v>
+        <v>1.9933340549468901</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4028,19 +4032,19 @@
         <v>2</v>
       </c>
       <c r="J83">
-        <v>2265.3995739771399</v>
+        <v>2268.7665103468198</v>
       </c>
       <c r="K83">
-        <v>2212.8004677510298</v>
+        <v>2215.3079035547798</v>
       </c>
       <c r="L83">
-        <v>187.93655985046999</v>
+        <v>185.36927460642099</v>
       </c>
       <c r="M83">
-        <v>283.48162221908501</v>
+        <v>178.36961984634399</v>
       </c>
       <c r="N83">
-        <v>1.49980497360229</v>
+        <v>1.54180407524108</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4072,19 +4076,19 @@
         <v>2</v>
       </c>
       <c r="J84">
-        <v>2904.8163929266102</v>
+        <v>2920.94926148286</v>
       </c>
       <c r="K84">
-        <v>2860.4786309180299</v>
+        <v>2870.0893454462698</v>
       </c>
       <c r="L84">
-        <v>279.42759489314898</v>
+        <v>277.63119389401601</v>
       </c>
       <c r="M84">
-        <v>340.90815997123701</v>
+        <v>178.137626886367</v>
       </c>
       <c r="N84">
-        <v>1.7080821990966699</v>
+        <v>1.5748760700225799</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -4116,19 +4120,19 @@
         <v>2</v>
       </c>
       <c r="J85">
-        <v>3435.6377688355601</v>
+        <v>3459.0548827103398</v>
       </c>
       <c r="K85">
-        <v>3618.3802994269099</v>
+        <v>3635.3150922226</v>
       </c>
       <c r="L85">
-        <v>573.061153003904</v>
+        <v>578.23064012765496</v>
       </c>
       <c r="M85">
-        <v>182.47144722938501</v>
+        <v>131.55616903305</v>
       </c>
       <c r="N85">
-        <v>1.28935003280639</v>
+        <v>1.4251279830932599</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -4160,19 +4164,19 @@
         <v>2</v>
       </c>
       <c r="J86">
-        <v>4238.84220102171</v>
+        <v>4253.5919799195299</v>
       </c>
       <c r="K86">
-        <v>4200.3970355576903</v>
+        <v>4216.0674042496703</v>
       </c>
       <c r="L86">
-        <v>367.70872790169</v>
+        <v>365.100472933557</v>
       </c>
       <c r="M86">
-        <v>244.62016725540099</v>
+        <v>240.77669620513899</v>
       </c>
       <c r="N86">
-        <v>1.59977602958679</v>
+        <v>1.9954986572265601</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -4204,19 +4208,19 @@
         <v>2</v>
       </c>
       <c r="J87">
-        <v>5462.8698604859101</v>
+        <v>5504.4981847666604</v>
       </c>
       <c r="K87">
-        <v>5365.6349633015898</v>
+        <v>5389.9700337167696</v>
       </c>
       <c r="L87">
-        <v>501.61919215285502</v>
+        <v>503.44751826573901</v>
       </c>
       <c r="M87">
-        <v>189.927205085754</v>
+        <v>235.15798997879</v>
       </c>
       <c r="N87">
-        <v>1.4837749004364</v>
+        <v>2.0434031486511199</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -4248,19 +4252,19 @@
         <v>2</v>
       </c>
       <c r="J88">
-        <v>6631.14089291853</v>
+        <v>6680.7462018332699</v>
       </c>
       <c r="K88">
-        <v>6871.6256709950603</v>
+        <v>6925.0849327794003</v>
       </c>
       <c r="L88">
-        <v>1010.7808537680399</v>
+        <v>1019.43077886943</v>
       </c>
       <c r="M88">
-        <v>280.48407793044998</v>
+        <v>187.00432205200099</v>
       </c>
       <c r="N88">
-        <v>1.7195019721984801</v>
+        <v>1.8552598953246999</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -4292,19 +4296,19 @@
         <v>2</v>
       </c>
       <c r="J89">
-        <v>6484.7950390239203</v>
+        <v>6510.5292401981096</v>
       </c>
       <c r="K89">
-        <v>6662.6538012073997</v>
+        <v>6713.1996836573899</v>
       </c>
       <c r="L89">
-        <v>620.03454460422802</v>
+        <v>626.76201559137405</v>
       </c>
       <c r="M89">
-        <v>299.171437978744</v>
+        <v>334.81972002983002</v>
       </c>
       <c r="N89">
-        <v>1.96833395957946</v>
+        <v>2.5842518806457502</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -4336,19 +4340,19 @@
         <v>2</v>
       </c>
       <c r="J90">
-        <v>8309.3815783226091</v>
+        <v>8396.6682343749308</v>
       </c>
       <c r="K90">
-        <v>8319.12567985854</v>
+        <v>8413.4831489109092</v>
       </c>
       <c r="L90">
-        <v>877.87220402463299</v>
+        <v>919.34156886026005</v>
       </c>
       <c r="M90">
-        <v>215.613170146942</v>
+        <v>207.165996074676</v>
       </c>
       <c r="N90">
-        <v>1.7376070022582999</v>
+        <v>2.1273779869079501</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -4380,19 +4384,19 @@
         <v>2</v>
       </c>
       <c r="J91">
-        <v>9883.1533182751791</v>
+        <v>9961.1380742103593</v>
       </c>
       <c r="K91">
-        <v>9968.7039696909596</v>
+        <v>9976.9207202754205</v>
       </c>
       <c r="L91">
-        <v>1339.6004735751501</v>
+        <v>1318.92290409719</v>
       </c>
       <c r="M91">
-        <v>306.914903163909</v>
+        <v>194.98811984062101</v>
       </c>
       <c r="N91">
-        <v>2.02897596359252</v>
+        <v>2.1605849266052202</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -4424,19 +4428,19 @@
         <v>2</v>
       </c>
       <c r="J92">
-        <v>2341.5120787881401</v>
+        <v>2344.3368664679801</v>
       </c>
       <c r="K92">
-        <v>2233.55149860458</v>
+        <v>2237.2982060193899</v>
       </c>
       <c r="L92">
-        <v>208.06899882317501</v>
+        <v>205.30769971749999</v>
       </c>
       <c r="M92">
-        <v>459.054688215255</v>
+        <v>258.781239986419</v>
       </c>
       <c r="N92">
-        <v>2.3852322101593</v>
+        <v>2.3374929428100502</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -4468,19 +4472,19 @@
         <v>2</v>
       </c>
       <c r="J93">
-        <v>2941.4430241711102</v>
+        <v>2954.25065891852</v>
       </c>
       <c r="K93">
-        <v>2819.1384847865402</v>
+        <v>2825.3587160828201</v>
       </c>
       <c r="L93">
-        <v>279.886020451457</v>
+        <v>281.16782907170898</v>
       </c>
       <c r="M93">
-        <v>309.209935188293</v>
+        <v>181.249975919723</v>
       </c>
       <c r="N93">
-        <v>2.3979232311248699</v>
+        <v>2.1538307666778498</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -4512,19 +4516,19 @@
         <v>2</v>
       </c>
       <c r="J94">
-        <v>3425.8734936031901</v>
+        <v>3446.0363881008998</v>
       </c>
       <c r="K94">
-        <v>3534.7753915512599</v>
+        <v>3562.73610390055</v>
       </c>
       <c r="L94">
-        <v>579.51742303561605</v>
+        <v>581.99892747844001</v>
       </c>
       <c r="M94">
-        <v>254.23241591453501</v>
+        <v>194.05462408065699</v>
       </c>
       <c r="N94">
-        <v>2.1352758407592698</v>
+        <v>2.0928320884704501</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -4556,19 +4560,19 @@
         <v>2</v>
       </c>
       <c r="J95">
-        <v>4260.7599288983001</v>
+        <v>4271.6321878273702</v>
       </c>
       <c r="K95">
-        <v>4179.2106945753803</v>
+        <v>4196.4280828361198</v>
       </c>
       <c r="L95">
-        <v>366.95139797587899</v>
+        <v>364.70406152952398</v>
       </c>
       <c r="M95">
-        <v>413.11932277679398</v>
+        <v>219.38100600242601</v>
       </c>
       <c r="N95">
-        <v>2.5758128166198699</v>
+        <v>2.4960160255432098</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -4600,19 +4604,19 @@
         <v>2</v>
       </c>
       <c r="J96">
-        <v>5432.16679065674</v>
+        <v>5453.81225944784</v>
       </c>
       <c r="K96">
-        <v>5271.5863914628299</v>
+        <v>5374.2690143973005</v>
       </c>
       <c r="L96">
-        <v>497.13505110834097</v>
+        <v>551.47231251568201</v>
       </c>
       <c r="M96">
-        <v>476.660197973251</v>
+        <v>226.95661497116001</v>
       </c>
       <c r="N96">
-        <v>2.9179799556732098</v>
+        <v>2.5601730346679599</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -4644,19 +4648,19 @@
         <v>2</v>
       </c>
       <c r="J97">
-        <v>6507.9379897285198</v>
+        <v>6551.5509161094897</v>
       </c>
       <c r="K97">
-        <v>6663.0241609547102</v>
+        <v>6685.8249505350896</v>
       </c>
       <c r="L97">
-        <v>988.81404680131698</v>
+        <v>980.51299636856902</v>
       </c>
       <c r="M97">
-        <v>292.444359064102</v>
+        <v>211.65870809555</v>
       </c>
       <c r="N97">
-        <v>2.4784190654754599</v>
+        <v>2.5025238990783598</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -4688,19 +4692,19 @@
         <v>2</v>
       </c>
       <c r="J98">
-        <v>6569.4058531630399</v>
+        <v>6591.0393921844097</v>
       </c>
       <c r="K98">
-        <v>6630.6486903145997</v>
+        <v>6675.8832690838299</v>
       </c>
       <c r="L98">
-        <v>624.25899404988604</v>
+        <v>629.28841348344497</v>
       </c>
       <c r="M98">
-        <v>286.61276078224103</v>
+        <v>254.213575839996</v>
       </c>
       <c r="N98">
-        <v>2.69271612167358</v>
+        <v>2.9565119743347101</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -4732,19 +4736,19 @@
         <v>2</v>
       </c>
       <c r="J99">
-        <v>8337.9036494318098</v>
+        <v>8383.9860416501797</v>
       </c>
       <c r="K99">
-        <v>8213.66311135668</v>
+        <v>8322.5768521841401</v>
       </c>
       <c r="L99">
-        <v>875.37129397543595</v>
+        <v>906.84202314140998</v>
       </c>
       <c r="M99">
-        <v>376.08304810523902</v>
+        <v>260.96389913558897</v>
       </c>
       <c r="N99">
-        <v>3.8787157535552899</v>
+        <v>3.08933401107788</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -4776,19 +4780,19 @@
         <v>2</v>
       </c>
       <c r="J100">
-        <v>9747.8918596934109</v>
+        <v>9805.9319673419395</v>
       </c>
       <c r="K100">
-        <v>9630.0963386768999</v>
+        <v>9839.4128088898706</v>
       </c>
       <c r="L100">
-        <v>1292.62419854375</v>
+        <v>1373.29535147557</v>
       </c>
       <c r="M100">
-        <v>317.13780307769701</v>
+        <v>152.44851493835401</v>
       </c>
       <c r="N100">
-        <v>2.5643012523651101</v>
+        <v>2.68913578987121</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -4820,19 +4824,19 @@
         <v>2</v>
       </c>
       <c r="J101">
-        <v>2297.8525043414302</v>
+        <v>2300.4749842772599</v>
       </c>
       <c r="K101">
-        <v>2208.4341742850202</v>
+        <v>2210.88871842047</v>
       </c>
       <c r="L101">
-        <v>189.95319452773199</v>
+        <v>187.30960112439499</v>
       </c>
       <c r="M101">
-        <v>332.93490004539399</v>
+        <v>295.14287900924597</v>
       </c>
       <c r="N101">
-        <v>2.74915099143981</v>
+        <v>3.1440019607543901</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -4864,19 +4868,19 @@
         <v>2</v>
       </c>
       <c r="J102">
-        <v>2931.9046686618799</v>
+        <v>2945.8673581408698</v>
       </c>
       <c r="K102">
-        <v>2827.7014300894198</v>
+        <v>2852.3770414534201</v>
       </c>
       <c r="L102">
-        <v>278.279753380898</v>
+        <v>285.12282279374602</v>
       </c>
       <c r="M102">
-        <v>384.89850378036499</v>
+        <v>289.13002324104298</v>
       </c>
       <c r="N102">
-        <v>3.0047409534454301</v>
+        <v>3.1872329711914</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -4908,19 +4912,19 @@
         <v>2</v>
       </c>
       <c r="J103">
-        <v>3444.0375292267699</v>
+        <v>3464.2873870242202</v>
       </c>
       <c r="K103">
-        <v>3577.41892631273</v>
+        <v>3596.2704770673799</v>
       </c>
       <c r="L103">
-        <v>580.56003730849704</v>
+        <v>578.98227255420102</v>
       </c>
       <c r="M103">
-        <v>268.06628084182699</v>
+        <v>260.44284009933398</v>
       </c>
       <c r="N103">
-        <v>2.6762328147888099</v>
+        <v>3.0905668735504102</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -4952,19 +4956,19 @@
         <v>2</v>
       </c>
       <c r="J104">
-        <v>4257.9700884888498</v>
+        <v>4269.5298963627502</v>
       </c>
       <c r="K104">
-        <v>4199.3516826781397</v>
+        <v>4214.7531872482896</v>
       </c>
       <c r="L104">
-        <v>370.219033870933</v>
+        <v>367.47179438291403</v>
       </c>
       <c r="M104">
-        <v>398.29696893692</v>
+        <v>467.59943580627402</v>
       </c>
       <c r="N104">
-        <v>3.2119760513305602</v>
+        <v>4.0356070995330802</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -4996,19 +5000,19 @@
         <v>2</v>
       </c>
       <c r="J105">
-        <v>5456.6891964885899</v>
+        <v>5490.8275871690703</v>
       </c>
       <c r="K105">
-        <v>5315.5385107555003</v>
+        <v>5353.6647529750499</v>
       </c>
       <c r="L105">
-        <v>502.99597440270099</v>
+        <v>504.39413137247698</v>
       </c>
       <c r="M105">
-        <v>770.99142694473198</v>
+        <v>433.10757684707602</v>
       </c>
       <c r="N105">
-        <v>4.17726397514343</v>
+        <v>3.9947440624236998</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -5040,19 +5044,19 @@
         <v>2</v>
       </c>
       <c r="J106">
-        <v>6562.7596686188099</v>
+        <v>6610.8031574367797</v>
       </c>
       <c r="K106">
-        <v>6735.3838387202504</v>
+        <v>6753.9036738098303</v>
       </c>
       <c r="L106">
-        <v>1001.70011126502</v>
+        <v>1002.09967111102</v>
       </c>
       <c r="M106">
-        <v>321.080037117004</v>
+        <v>329.16289401054303</v>
       </c>
       <c r="N106">
-        <v>3.15293884277343</v>
+        <v>3.6443960666656401</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -5084,19 +5088,19 @@
         <v>2</v>
       </c>
       <c r="J107">
-        <v>6533.2568013240798</v>
+        <v>6557.0518059289197</v>
       </c>
       <c r="K107">
-        <v>6657.4764925953996</v>
+        <v>6704.8336638650799</v>
       </c>
       <c r="L107">
-        <v>622.51096145192298</v>
+        <v>627.09245281356505</v>
       </c>
       <c r="M107">
-        <v>451.67072987556401</v>
+        <v>750.17091679573002</v>
       </c>
       <c r="N107">
-        <v>4.2461240291595397</v>
+        <v>5.14784383773803</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -5128,19 +5132,19 @@
         <v>2</v>
       </c>
       <c r="J108">
-        <v>8347.1685437155702</v>
+        <v>8396.0903034292405</v>
       </c>
       <c r="K108">
-        <v>8324.6806586422699</v>
+        <v>8315.1187122811207</v>
       </c>
       <c r="L108">
-        <v>913.50904768663497</v>
+        <v>892.72495743959803</v>
       </c>
       <c r="M108">
-        <v>617.94475102424599</v>
+        <v>459.920213937759</v>
       </c>
       <c r="N108">
-        <v>3.9560689926147399</v>
+        <v>4.6099879741668701</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -5172,19 +5176,19 @@
         <v>2</v>
       </c>
       <c r="J109">
-        <v>9803.0877054159591</v>
+        <v>9866.7634765839703</v>
       </c>
       <c r="K109">
-        <v>9784.6956532466793</v>
+        <v>9828.0889976073304</v>
       </c>
       <c r="L109">
-        <v>1333.4930760828199</v>
+        <v>1336.5735750972201</v>
       </c>
       <c r="M109">
-        <v>495.84429597854597</v>
+        <v>322.185586929321</v>
       </c>
       <c r="N109">
-        <v>3.7080271244049001</v>
+        <v>3.9242582321166899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>